<commit_message>
Added graphs to the rmark that breakdown each sites species differences for families with lots of species.  Also added 2 boat arrival times to the soundsampling excel.
</commit_message>
<xml_diff>
--- a/Project_Plan/Fish_Survey_SoundSampling.xlsx
+++ b/Project_Plan/Fish_Survey_SoundSampling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sdimo\Documents\GitHub\Sean_Acoustics\Project_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C058DC3-93C8-4C24-8DE4-250676D321A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE70FF2-C5CD-48FD-BFBF-14F94A20E703}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="4980" activeTab="1" xr2:uid="{8A30EA2C-F094-41D4-96C3-40CC1E2612F6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Site</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>No recording</t>
+  </si>
+  <si>
+    <t>Deployed 11:15</t>
   </si>
 </sst>
 </file>
@@ -105,9 +108,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -155,26 +158,26 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,97 +529,97 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A11:G11"/>
     <mergeCell ref="A4:G6"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -626,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B971E4B0-C69A-4677-A3D6-70EFB130AF14}">
   <dimension ref="A4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="132" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -638,360 +641,364 @@
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="11.46484375" customWidth="1"/>
     <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" customWidth="1"/>
+    <col min="8" max="8" width="15.06640625" customWidth="1"/>
     <col min="9" max="9" width="14.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>43280</v>
+        <v>43270</v>
       </c>
       <c r="C6" s="1">
-        <v>0.5541666666666667</v>
+        <v>0.57222222222222219</v>
       </c>
       <c r="D6" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E6" s="1">
-        <v>0.53125</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F6" s="1">
-        <v>0.60416666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="G6" s="1">
-        <v>0.61458333333333337</v>
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.55277777777777781</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>43273</v>
+        <v>43268</v>
       </c>
       <c r="C7" s="1">
-        <v>0.47986111111111113</v>
+        <v>0.51458333333333328</v>
       </c>
       <c r="D7" s="1">
-        <v>0.44791666666666669</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E7" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="F7" s="1">
-        <v>0.53125</v>
+        <v>0.5625</v>
       </c>
       <c r="G7" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="3">
-        <v>40</v>
+      <c r="A8">
+        <v>5</v>
       </c>
       <c r="B8" s="5">
-        <v>43272</v>
+        <v>42925</v>
       </c>
       <c r="C8" s="1">
-        <v>0.71527777777777779</v>
+        <v>0.3576388888888889</v>
       </c>
       <c r="D8" s="1">
-        <v>0.67708333333333337</v>
+        <v>0.32291666666666669</v>
       </c>
       <c r="E8" s="1">
-        <v>0.6875</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F8" s="1">
-        <v>0.76041666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="G8" s="1">
-        <v>0.77083333333333337</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" s="5">
-        <v>43270</v>
+        <v>42923</v>
       </c>
       <c r="C9" s="1">
-        <v>0.57222222222222219</v>
+        <v>0.5805555555555556</v>
       </c>
       <c r="D9" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="E9" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="F9" s="1">
-        <v>0.625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="G9" s="1">
-        <v>0.63541666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>43268</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.63402777777777775</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43266</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.53125</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5">
+        <v>42927</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5">
+        <v>42926</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.70277777777777783</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>32</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B14" s="5">
+        <v>43273</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
+        <v>32</v>
+      </c>
+      <c r="B15" s="5">
         <v>43270</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C15" s="1">
         <v>0.72361111111111109</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D15" s="1">
         <v>0.6875</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E15" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F15" s="1">
         <v>0.78125</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G15" s="1">
         <v>0.79166666666666663</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
-        <v>35</v>
-      </c>
-      <c r="B11" s="5">
-        <v>43269</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.57638888888888895</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.55208333333333337</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.63541666666666663</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
-        <v>5</v>
-      </c>
-      <c r="B12" s="5">
-        <v>43268</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.51458333333333328</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.5625</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
-        <v>8</v>
-      </c>
-      <c r="B13" s="5">
-        <v>43268</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.63402777777777775</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.6875</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="10">
-        <v>8</v>
-      </c>
-      <c r="B14" s="11">
-        <v>43266</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0.47430555555555554</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0.4375</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0.44791666666666669</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0.53125</v>
-      </c>
-      <c r="G14" s="12">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>35</v>
-      </c>
-      <c r="B15" s="5">
-        <v>43266</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.67638888888888893</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.73958333333333337</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5">
-        <v>42932</v>
+        <v>42930</v>
       </c>
       <c r="C16" s="1">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5">
+        <v>43269</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E17" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D16" s="1">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.61458333333333337</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5">
-        <v>42930</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.6743055555555556</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="F17" s="1">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E17" s="1">
+      <c r="G17" s="1">
         <v>0.64583333333333337</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.73958333333333337</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5">
-        <v>42927</v>
+        <v>43266</v>
       </c>
       <c r="C18" s="1">
-        <v>0.44861111111111113</v>
+        <v>0.67638888888888893</v>
       </c>
       <c r="D18" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="E18" s="1">
-        <v>0.42708333333333331</v>
+        <v>0.65625</v>
       </c>
       <c r="F18" s="1">
-        <v>0.5</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="G18" s="1">
-        <v>0.51041666666666663</v>
+        <v>0.73958333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1018,77 +1025,77 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>8</v>
+      <c r="A20" s="3">
+        <v>40</v>
       </c>
       <c r="B20" s="5">
-        <v>42926</v>
+        <v>43280</v>
       </c>
       <c r="C20" s="1">
-        <v>0.70277777777777783</v>
+        <v>0.5541666666666667</v>
       </c>
       <c r="D20" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E20" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="3">
+        <v>40</v>
+      </c>
+      <c r="B21" s="5">
+        <v>43272</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="D21" s="1">
         <v>0.67708333333333337</v>
       </c>
-      <c r="F20" s="1">
+      <c r="E21" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="F21" s="1">
         <v>0.76041666666666663</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G21" s="1">
         <v>0.77083333333333337</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21" s="5">
-        <v>42925</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.3576388888888889</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.32291666666666669</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5">
-        <v>42923</v>
+        <v>42932</v>
       </c>
       <c r="C22" s="1">
-        <v>0.5805555555555556</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="D22" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E22" s="1">
-        <v>0.5625</v>
+        <v>0.53125</v>
       </c>
       <c r="F22" s="1">
-        <v>0.63541666666666663</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="G22" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.61458333333333337</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C22">
-    <sortCondition descending="1" ref="B5"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G22">
+    <sortCondition ref="A6"/>
   </sortState>
   <mergeCells count="9">
     <mergeCell ref="A4:A5"/>

</xml_diff>